<commit_message>
import export asset name, export depre, test down
</commit_message>
<xml_diff>
--- a/public/template/TemplateAssetName.xlsx
+++ b/public/template/TemplateAssetName.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Asset Sub Class ID</t>
   </si>
@@ -45,13 +42,19 @@
   </si>
   <si>
     <t>LVA</t>
+  </si>
+  <si>
+    <t>Build Permanent-Housing</t>
+  </si>
+  <si>
+    <t>Asset Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,8 +77,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +96,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -113,24 +128,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,47 +427,65 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="19.21875" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3304</v>
+      </c>
+      <c r="D2" s="3">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update UI form, update AssetName Import, fix status sse
</commit_message>
<xml_diff>
--- a/public/template/TemplateAssetName.xlsx
+++ b/public/template/TemplateAssetName.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Asset Grouping</t>
   </si>
@@ -33,12 +33,6 @@
   </si>
   <si>
     <t>Fiscal Life</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>LVA</t>
   </si>
   <si>
     <t>Build Permanent-Housing</t>
@@ -427,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,16 +434,14 @@
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="19.21875" customWidth="1"/>
     <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -460,19 +452,13 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>3304</v>
@@ -482,12 +468,6 @@
       </c>
       <c r="E2" s="3">
         <v>20</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1000</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>